<commit_message>
Emerging Tech, FinTech Q32025 Update
</commit_message>
<xml_diff>
--- a/Emerging Tech/MBLY_MODEL.xlsx
+++ b/Emerging Tech/MBLY_MODEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Emerging Tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D247C01F-03CE-4777-9126-8867E8513B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAEC113-5F78-427C-9408-AA7D6AF8A9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="154">
   <si>
     <t>Price</t>
   </si>
@@ -430,6 +430,179 @@
   </si>
   <si>
     <t>Automatic lane-change, traffic-jam assist, blind-spot and cut-in avoidance, point-to-point nav, evasive manoeuvre assist, surround-view parking</t>
+  </si>
+  <si>
+    <t>P/Sales</t>
+  </si>
+  <si>
+    <t>P/Book</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>EV/R</t>
+  </si>
+  <si>
+    <t>Trl P/E</t>
+  </si>
+  <si>
+    <t>Fwd P/E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EBITDA </t>
+  </si>
+  <si>
+    <t>Diluted EPS TTM</t>
+  </si>
+  <si>
+    <t>Metric (TTM unless noted)</t>
+  </si>
+  <si>
+    <t>Mobileye</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>Qualcomm</t>
+  </si>
+  <si>
+    <t>Ambarella</t>
+  </si>
+  <si>
+    <t>Aptiv</t>
+  </si>
+  <si>
+    <t>Baidu</t>
+  </si>
+  <si>
+    <t>Forward P/E</t>
+  </si>
+  <si>
+    <t>33.1 × (Finviz)</t>
+  </si>
+  <si>
+    <t>30.2 × (Finviz)</t>
+  </si>
+  <si>
+    <t>12.2 × (Finviz)</t>
+  </si>
+  <si>
+    <t>200 × (Finviz)</t>
+  </si>
+  <si>
+    <t>8.1 × (Finviz)</t>
+  </si>
+  <si>
+    <t>9.2 × (Finviz)</t>
+  </si>
+  <si>
+    <t>EV / EBITDA</t>
+  </si>
+  <si>
+    <t>79.7 × (Finviz)</t>
+  </si>
+  <si>
+    <t>48.5 × (Finviz)</t>
+  </si>
+  <si>
+    <t>11.7 × (Finviz)</t>
+  </si>
+  <si>
+    <t>n/m (-) (Finviz)</t>
+  </si>
+  <si>
+    <t>6.7 × (Finviz)</t>
+  </si>
+  <si>
+    <t>5.6 × (Finviz)</t>
+  </si>
+  <si>
+    <t>Price / Sales</t>
+  </si>
+  <si>
+    <t>6.0 × (Finviz)</t>
+  </si>
+  <si>
+    <t>29.1 × (Finviz)</t>
+  </si>
+  <si>
+    <t>3.7 × (Finviz)</t>
+  </si>
+  <si>
+    <t>8.6 × (Finviz)</t>
+  </si>
+  <si>
+    <t>0.7 × (Finviz)</t>
+  </si>
+  <si>
+    <t>1.3 × (Finviz)</t>
+  </si>
+  <si>
+    <t>+18 % (EyeQ6 ramp)</t>
+  </si>
+  <si>
+    <t>+30 % auto seg.; &gt;50 % group</t>
+  </si>
+  <si>
+    <t>+25 % auto seg.</t>
+  </si>
+  <si>
+    <t>+45 % (edge-AI start-up wins)</t>
+  </si>
+  <si>
+    <t>low-single-digits</t>
+  </si>
+  <si>
+    <r>
+      <t>Growth context</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (FY-25e rev. Y/Y)</t>
+    </r>
+  </si>
+  <si>
+    <t>Fiscal year</t>
+  </si>
+  <si>
+    <t>Automotive revenue</t>
+  </si>
+  <si>
+    <t>Source / notes</t>
+  </si>
+  <si>
+    <t>$3.96B</t>
+  </si>
+  <si>
+    <t>QCT segment table in Qualcomm’s FY2025 10-K: Automotive $3,957M out of QCT’s $38.37B. (Q4 Capital)</t>
+  </si>
+  <si>
+    <t>$2.91B</t>
+  </si>
+  <si>
+    <t>Same 10-K table shows Automotive $2,910M for FY2024. (Q4 Capital)</t>
+  </si>
+  <si>
+    <t>$1.90B</t>
+  </si>
+  <si>
+    <t>FY22–FY23 “QCT Revenue Streams” slide shows Automotive rising from $1.5B (FY22) to $1.9B (FY23). (device.report)</t>
+  </si>
+  <si>
+    <t>$1.50B</t>
+  </si>
+  <si>
+    <t>Same FY22–FY23 slide: Automotive $1.5B in FY22. (device.report)</t>
+  </si>
+  <si>
+    <t>Qualcom</t>
   </si>
 </sst>
 </file>
@@ -440,13 +613,19 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -626,59 +805,69 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1015,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB11C10-986F-41A4-B3DD-2A72A923BC11}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1049,10 +1238,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1">
-        <v>14.08</v>
+        <v>11.38</v>
       </c>
       <c r="C4" s="2">
-        <v>45872</v>
+        <v>45981</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1060,10 +1249,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>806</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>814</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1072,7 +1261,7 @@
       </c>
       <c r="B6" s="1">
         <f xml:space="preserve"> B4 * B5</f>
-        <v>11348.48</v>
+        <v>9263.3200000000015</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1080,7 +1269,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="1">
-        <v>1710</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1088,13 +1277,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="1">
-        <v>2.1</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1103,13 +1292,71 @@
       </c>
       <c r="B9" s="1">
         <f>B6 - B7 + B8</f>
-        <v>9694.48</v>
+        <v>7574.3200000000015</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="1">
-        <v>14.8</v>
+        <v>14.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1122,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:Z77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1142,7 +1389,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1150,80 +1397,80 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="N2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="O2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="P2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="R2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="S2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="T2" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27">
         <v>378</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="27">
         <v>441</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="27">
         <v>432</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="27">
         <v>543</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="27">
         <v>438</v>
       </c>
       <c r="I3" s="1">
@@ -1252,6 +1499,9 @@
       </c>
       <c r="Q3" s="1">
         <v>481</v>
+      </c>
+      <c r="R3" s="1">
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1300,6 +1550,9 @@
       <c r="Q4" s="1">
         <v>9.6999999999999993</v>
       </c>
+      <c r="R4" s="1">
+        <v>9.1999999999999993</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1347,16 +1600,19 @@
       <c r="Q5" s="1">
         <v>49.7</v>
       </c>
+      <c r="R5" s="1">
+        <v>51.7</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:20" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -1406,43 +1662,45 @@
       <c r="Q7" s="4">
         <v>506</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="4">
+        <v>504</v>
+      </c>
       <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27">
         <v>218</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="27">
         <v>231</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="28">
         <v>233</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="28">
         <v>265</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="28">
         <v>251</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="28">
         <v>230</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="28">
         <v>258</v>
       </c>
       <c r="K8" s="1">
         <v>293</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="28">
         <v>185</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="28">
         <v>230</v>
       </c>
       <c r="N8" s="1">
@@ -1456,6 +1714,9 @@
       </c>
       <c r="Q8" s="1">
         <v>254</v>
+      </c>
+      <c r="R8" s="1">
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1465,7 +1726,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <f t="shared" ref="D9:Q9" si="0">D7 -D8</f>
+        <f t="shared" ref="D9:R9" si="0">D7 -D8</f>
         <v>176</v>
       </c>
       <c r="E9" s="4">
@@ -1520,10 +1781,14 @@
         <f t="shared" si="0"/>
         <v>252</v>
       </c>
+      <c r="R9" s="4">
+        <f t="shared" si="0"/>
+        <v>243</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="18"/>
@@ -1569,10 +1834,13 @@
       <c r="Q10" s="18">
         <v>282</v>
       </c>
+      <c r="R10" s="1">
+        <v>304</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="18"/>
@@ -1618,53 +1886,59 @@
       <c r="Q11" s="18">
         <v>25</v>
       </c>
+      <c r="R11" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27">
         <v>7</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="27">
         <v>11</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="28">
         <v>9</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="28">
         <v>23</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="28">
         <v>20</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="28">
         <v>17</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="28">
         <v>18</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="28">
         <v>18</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="28">
         <v>15</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="28">
         <v>19</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="28">
         <v>18</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="28">
         <v>18</v>
       </c>
       <c r="P12" s="1">
         <v>18</v>
       </c>
-      <c r="Q12" s="31">
+      <c r="Q12" s="28">
+        <v>19</v>
+      </c>
+      <c r="R12" s="1">
         <v>19</v>
       </c>
     </row>
@@ -1728,6 +2002,10 @@
         <f>Q9-SUM(Q10:Q12)</f>
         <v>-74</v>
       </c>
+      <c r="R13" s="4">
+        <f>R9-SUM(R10:R12)</f>
+        <v>-109</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
@@ -1739,31 +2017,31 @@
       <c r="E14" s="1">
         <v>8</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="28">
         <v>-30</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="28">
         <v>34</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="28">
         <v>-73</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="28">
         <v>-18</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="28">
         <v>23</v>
       </c>
       <c r="K14" s="1">
         <v>84</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="28">
         <v>-221</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="28">
         <v>-81</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="28">
         <v>-2793</v>
       </c>
       <c r="O14" s="1">
@@ -1774,6 +2052,9 @@
       </c>
       <c r="Q14" s="1">
         <v>-61</v>
+      </c>
+      <c r="R14" s="1">
+        <v>-92</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -1786,31 +2067,31 @@
       <c r="E15" s="1">
         <v>15</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="28">
         <v>15</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="28">
         <v>4</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="28">
         <v>6</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="28">
         <v>10</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="28">
         <v>6</v>
       </c>
       <c r="K15" s="1">
         <v>21</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="28">
         <v>-3</v>
       </c>
       <c r="M15" s="1">
         <v>5</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="28">
         <v>-78</v>
       </c>
       <c r="O15" s="1">
@@ -1821,6 +2102,9 @@
       </c>
       <c r="Q15" s="1">
         <v>6</v>
+      </c>
+      <c r="R15" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:20" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -1883,56 +2167,63 @@
         <f>Q14-Q15</f>
         <v>-67</v>
       </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="5">
+        <f>R14-R15</f>
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32">
+      <c r="C17" s="29"/>
+      <c r="D17" s="29">
         <v>-0.08</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="29">
         <v>-0.01</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="29">
         <v>-0.06</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="29">
         <v>0.04</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="29">
         <v>-0.1</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="29">
         <v>-0.04</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="29">
         <v>0.02</v>
       </c>
       <c r="K17" s="1">
         <v>0.08</v>
       </c>
-      <c r="L17" s="32">
+      <c r="L17" s="29">
         <v>-0.27</v>
       </c>
-      <c r="M17" s="32">
+      <c r="M17" s="29">
         <v>-0.11</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="29">
         <v>-3.35</v>
       </c>
-      <c r="O17" s="32">
+      <c r="O17" s="29">
         <v>-0.09</v>
       </c>
       <c r="P17" s="1">
         <v>-0.13</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="29">
         <v>-0.08</v>
       </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="1">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1951,22 +2242,22 @@
       <c r="H18" s="1">
         <v>-0.1</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="28">
         <v>-0.04</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="28">
         <v>0.02</v>
       </c>
       <c r="K18" s="1">
         <v>0.08</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="28">
         <v>-0.27</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="28">
         <v>-0.11</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="28">
         <v>-3.35</v>
       </c>
       <c r="O18" s="1">
@@ -1978,8 +2269,11 @@
       <c r="Q18" s="1">
         <v>-0.08</v>
       </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R18" s="1">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
@@ -2004,7 +2298,7 @@
         <v>-1.3043478260869601E-2</v>
       </c>
       <c r="J20" s="6">
-        <f t="shared" ref="J20:Q20" si="7">(J7/F7) - 1</f>
+        <f t="shared" ref="J20:R20" si="7">(J7/F7) - 1</f>
         <v>0.17777777777777781</v>
       </c>
       <c r="K20" s="6">
@@ -2035,8 +2329,12 @@
         <f t="shared" si="7"/>
         <v>0.15261958997722092</v>
       </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R20" s="6">
+        <f t="shared" si="7"/>
+        <v>3.7037037037036979E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
@@ -2052,7 +2350,7 @@
         <v>-2.1739130434782594E-2</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" ref="G21:Q21" si="10" xml:space="preserve"> (G7/F7) - 1</f>
+        <f t="shared" ref="G21:R21" si="10" xml:space="preserve"> (G7/F7) - 1</f>
         <v>0.25555555555555554</v>
       </c>
       <c r="H21" s="6">
@@ -2095,8 +2393,12 @@
         <f t="shared" si="10"/>
         <v>0.15525114155251152</v>
       </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R21" s="6">
+        <f t="shared" si="10"/>
+        <v>-3.9525691699604515E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="F22" s="6"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -2109,7 +2411,7 @@
       <c r="O22" s="7"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
@@ -2155,8 +2457,11 @@
       <c r="Q23" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R23" s="6">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>55</v>
       </c>
@@ -2202,8 +2507,11 @@
       <c r="Q24" s="6">
         <v>0.69</v>
       </c>
-    </row>
-    <row r="25" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R24" s="6">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
@@ -2249,8 +2557,11 @@
       <c r="Q25" s="6">
         <v>-0.15</v>
       </c>
-    </row>
-    <row r="26" spans="2:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="R25" s="6">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>48</v>
       </c>
@@ -2296,37 +2607,40 @@
       <c r="Q26" s="8">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="28" spans="2:17" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
+      <c r="R26" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B28" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33">
+      <c r="C28" s="30"/>
+      <c r="D28" s="30">
         <v>51</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="30">
         <v>182</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="31">
         <v>162</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="31">
         <v>151</v>
       </c>
-      <c r="H28" s="34">
+      <c r="H28" s="31">
         <v>172</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28" s="31">
         <v>26</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="31">
         <v>88</v>
       </c>
-      <c r="K28" s="34">
+      <c r="K28" s="31">
         <v>109</v>
       </c>
-      <c r="L28" s="34">
+      <c r="L28" s="31">
         <v>88</v>
       </c>
       <c r="M28" s="9">
@@ -2344,40 +2658,43 @@
       <c r="Q28" s="9">
         <v>213</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="30" t="s">
+      <c r="R28" s="9">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27">
         <v>27</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="27">
         <v>26</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="28">
         <v>26</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="28">
         <v>32</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H29" s="28">
         <v>26</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="28">
         <v>32</v>
       </c>
-      <c r="J29" s="31">
+      <c r="J29" s="28">
         <v>17</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="28">
         <v>23</v>
       </c>
-      <c r="L29" s="31">
+      <c r="L29" s="28">
         <v>22</v>
       </c>
-      <c r="M29" s="31">
+      <c r="M29" s="28">
         <v>24</v>
       </c>
       <c r="N29" s="1">
@@ -2392,9 +2709,12 @@
       <c r="Q29" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="2:17" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="33" t="s">
+      <c r="R29" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="9">
@@ -2453,19 +2773,23 @@
         <f>Q28-Q29</f>
         <v>199</v>
       </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="30"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="30" t="s">
+      <c r="R30" s="9">
+        <f>R28-R29</f>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B32" s="27" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2520,9 +2844,13 @@
         <f>IF(M30=0,IF(Q30=0,0,NA()),(Q30-M30)/ABS(M30))</f>
         <v>32.166666666666664</v>
       </c>
+      <c r="R32" s="6">
+        <f>IF(N30=0,IF(R30=0,0,NA()),(R30-N30)/ABS(N30))</f>
+        <v>0.375</v>
+      </c>
     </row>
     <row r="34" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
+      <c r="B34" s="27"/>
       <c r="G34" s="11"/>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.2">
@@ -2721,301 +3049,301 @@
       <c r="B54" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
-      <c r="N54" s="35"/>
-      <c r="O54" s="35"/>
-      <c r="P54" s="35"/>
-      <c r="Q54" s="35"/>
-      <c r="R54" s="35"/>
-      <c r="S54" s="35"/>
-      <c r="T54" s="35"/>
-      <c r="U54" s="35"/>
-      <c r="V54" s="35"/>
-      <c r="W54" s="35"/>
-      <c r="X54" s="35"/>
-      <c r="Y54" s="35"/>
-      <c r="Z54" s="36"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="32"/>
+      <c r="N54" s="32"/>
+      <c r="O54" s="32"/>
+      <c r="P54" s="32"/>
+      <c r="Q54" s="32"/>
+      <c r="R54" s="32"/>
+      <c r="S54" s="32"/>
+      <c r="T54" s="32"/>
+      <c r="U54" s="32"/>
+      <c r="V54" s="32"/>
+      <c r="W54" s="32"/>
+      <c r="X54" s="32"/>
+      <c r="Y54" s="32"/>
+      <c r="Z54" s="33"/>
     </row>
     <row r="55" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="16"/>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="35"/>
-      <c r="N55" s="35"/>
-      <c r="O55" s="35"/>
-      <c r="P55" s="35"/>
-      <c r="Q55" s="35"/>
-      <c r="R55" s="35"/>
-      <c r="S55" s="35"/>
-      <c r="T55" s="35"/>
-      <c r="U55" s="35"/>
-      <c r="V55" s="35"/>
-      <c r="W55" s="35"/>
-      <c r="X55" s="35"/>
-      <c r="Y55" s="35"/>
-      <c r="Z55" s="36"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32"/>
+      <c r="L55" s="32"/>
+      <c r="M55" s="32"/>
+      <c r="N55" s="32"/>
+      <c r="O55" s="32"/>
+      <c r="P55" s="32"/>
+      <c r="Q55" s="32"/>
+      <c r="R55" s="32"/>
+      <c r="S55" s="32"/>
+      <c r="T55" s="32"/>
+      <c r="U55" s="32"/>
+      <c r="V55" s="32"/>
+      <c r="W55" s="32"/>
+      <c r="X55" s="32"/>
+      <c r="Y55" s="32"/>
+      <c r="Z55" s="33"/>
     </row>
     <row r="56" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="16"/>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="35"/>
-      <c r="P56" s="35"/>
-      <c r="Q56" s="35"/>
-      <c r="R56" s="35"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="35"/>
-      <c r="U56" s="35"/>
-      <c r="V56" s="35"/>
-      <c r="W56" s="35"/>
-      <c r="X56" s="35"/>
-      <c r="Y56" s="35"/>
-      <c r="Z56" s="36"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="32"/>
+      <c r="L56" s="32"/>
+      <c r="M56" s="32"/>
+      <c r="N56" s="32"/>
+      <c r="O56" s="32"/>
+      <c r="P56" s="32"/>
+      <c r="Q56" s="32"/>
+      <c r="R56" s="32"/>
+      <c r="S56" s="32"/>
+      <c r="T56" s="32"/>
+      <c r="U56" s="32"/>
+      <c r="V56" s="32"/>
+      <c r="W56" s="32"/>
+      <c r="X56" s="32"/>
+      <c r="Y56" s="32"/>
+      <c r="Z56" s="33"/>
     </row>
     <row r="57" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="16"/>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="35"/>
-      <c r="K57" s="35"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="35"/>
-      <c r="N57" s="35"/>
-      <c r="O57" s="35"/>
-      <c r="P57" s="35"/>
-      <c r="Q57" s="35"/>
-      <c r="R57" s="35"/>
-      <c r="S57" s="35"/>
-      <c r="T57" s="35"/>
-      <c r="U57" s="35"/>
-      <c r="V57" s="35"/>
-      <c r="W57" s="35"/>
-      <c r="X57" s="35"/>
-      <c r="Y57" s="35"/>
-      <c r="Z57" s="36"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="32"/>
+      <c r="L57" s="32"/>
+      <c r="M57" s="32"/>
+      <c r="N57" s="32"/>
+      <c r="O57" s="32"/>
+      <c r="P57" s="32"/>
+      <c r="Q57" s="32"/>
+      <c r="R57" s="32"/>
+      <c r="S57" s="32"/>
+      <c r="T57" s="32"/>
+      <c r="U57" s="32"/>
+      <c r="V57" s="32"/>
+      <c r="W57" s="32"/>
+      <c r="X57" s="32"/>
+      <c r="Y57" s="32"/>
+      <c r="Z57" s="33"/>
     </row>
     <row r="58" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="16"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35"/>
-      <c r="O58" s="35"/>
-      <c r="P58" s="35"/>
-      <c r="Q58" s="35"/>
-      <c r="R58" s="35"/>
-      <c r="S58" s="35"/>
-      <c r="T58" s="35"/>
-      <c r="U58" s="35"/>
-      <c r="V58" s="35"/>
-      <c r="W58" s="35"/>
-      <c r="X58" s="35"/>
-      <c r="Y58" s="35"/>
-      <c r="Z58" s="36"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
+      <c r="O58" s="32"/>
+      <c r="P58" s="32"/>
+      <c r="Q58" s="32"/>
+      <c r="R58" s="32"/>
+      <c r="S58" s="32"/>
+      <c r="T58" s="32"/>
+      <c r="U58" s="32"/>
+      <c r="V58" s="32"/>
+      <c r="W58" s="32"/>
+      <c r="X58" s="32"/>
+      <c r="Y58" s="32"/>
+      <c r="Z58" s="33"/>
     </row>
     <row r="59" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="35"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="35"/>
-      <c r="P59" s="35"/>
-      <c r="Q59" s="35"/>
-      <c r="R59" s="35"/>
-      <c r="S59" s="35"/>
-      <c r="T59" s="35"/>
-      <c r="U59" s="35"/>
-      <c r="V59" s="35"/>
-      <c r="W59" s="35"/>
-      <c r="X59" s="35"/>
-      <c r="Y59" s="35"/>
-      <c r="Z59" s="36"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
+      <c r="O59" s="32"/>
+      <c r="P59" s="32"/>
+      <c r="Q59" s="32"/>
+      <c r="R59" s="32"/>
+      <c r="S59" s="32"/>
+      <c r="T59" s="32"/>
+      <c r="U59" s="32"/>
+      <c r="V59" s="32"/>
+      <c r="W59" s="32"/>
+      <c r="X59" s="32"/>
+      <c r="Y59" s="32"/>
+      <c r="Z59" s="33"/>
     </row>
     <row r="60" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="35"/>
-      <c r="Q60" s="35"/>
-      <c r="R60" s="35"/>
-      <c r="S60" s="35"/>
-      <c r="T60" s="35"/>
-      <c r="U60" s="35"/>
-      <c r="V60" s="35"/>
-      <c r="W60" s="35"/>
-      <c r="X60" s="35"/>
-      <c r="Y60" s="35"/>
-      <c r="Z60" s="36"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="32"/>
+      <c r="P60" s="32"/>
+      <c r="Q60" s="32"/>
+      <c r="R60" s="32"/>
+      <c r="S60" s="32"/>
+      <c r="T60" s="32"/>
+      <c r="U60" s="32"/>
+      <c r="V60" s="32"/>
+      <c r="W60" s="32"/>
+      <c r="X60" s="32"/>
+      <c r="Y60" s="32"/>
+      <c r="Z60" s="33"/>
     </row>
     <row r="61" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-      <c r="M61" s="35"/>
-      <c r="N61" s="35"/>
-      <c r="O61" s="35"/>
-      <c r="P61" s="35"/>
-      <c r="Q61" s="35"/>
-      <c r="R61" s="35"/>
-      <c r="S61" s="35"/>
-      <c r="T61" s="35"/>
-      <c r="U61" s="35"/>
-      <c r="V61" s="35"/>
-      <c r="W61" s="35"/>
-      <c r="X61" s="35"/>
-      <c r="Y61" s="35"/>
-      <c r="Z61" s="36"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="32"/>
+      <c r="J61" s="32"/>
+      <c r="K61" s="32"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="32"/>
+      <c r="P61" s="32"/>
+      <c r="Q61" s="32"/>
+      <c r="R61" s="32"/>
+      <c r="S61" s="32"/>
+      <c r="T61" s="32"/>
+      <c r="U61" s="32"/>
+      <c r="V61" s="32"/>
+      <c r="W61" s="32"/>
+      <c r="X61" s="32"/>
+      <c r="Y61" s="32"/>
+      <c r="Z61" s="33"/>
     </row>
     <row r="62" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="35"/>
-      <c r="J62" s="35"/>
-      <c r="K62" s="35"/>
-      <c r="L62" s="35"/>
-      <c r="M62" s="35"/>
-      <c r="N62" s="35"/>
-      <c r="O62" s="35"/>
-      <c r="P62" s="35"/>
-      <c r="Q62" s="35"/>
-      <c r="R62" s="35"/>
-      <c r="S62" s="35"/>
-      <c r="T62" s="35"/>
-      <c r="U62" s="35"/>
-      <c r="V62" s="35"/>
-      <c r="W62" s="35"/>
-      <c r="X62" s="35"/>
-      <c r="Y62" s="35"/>
-      <c r="Z62" s="36"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
+      <c r="J62" s="32"/>
+      <c r="K62" s="32"/>
+      <c r="L62" s="32"/>
+      <c r="M62" s="32"/>
+      <c r="N62" s="32"/>
+      <c r="O62" s="32"/>
+      <c r="P62" s="32"/>
+      <c r="Q62" s="32"/>
+      <c r="R62" s="32"/>
+      <c r="S62" s="32"/>
+      <c r="T62" s="32"/>
+      <c r="U62" s="32"/>
+      <c r="V62" s="32"/>
+      <c r="W62" s="32"/>
+      <c r="X62" s="32"/>
+      <c r="Y62" s="32"/>
+      <c r="Z62" s="33"/>
     </row>
     <row r="63" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="C63" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
-      <c r="O63" s="35"/>
-      <c r="P63" s="35"/>
-      <c r="Q63" s="35"/>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35"/>
-      <c r="T63" s="35"/>
-      <c r="U63" s="35"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
-      <c r="Z63" s="36"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
+      <c r="O63" s="32"/>
+      <c r="P63" s="32"/>
+      <c r="Q63" s="32"/>
+      <c r="R63" s="32"/>
+      <c r="S63" s="32"/>
+      <c r="T63" s="32"/>
+      <c r="U63" s="32"/>
+      <c r="V63" s="32"/>
+      <c r="W63" s="32"/>
+      <c r="X63" s="32"/>
+      <c r="Y63" s="32"/>
+      <c r="Z63" s="33"/>
     </row>
     <row r="64" spans="2:26" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
@@ -3169,139 +3497,279 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD6AACC-FEA2-4C5B-AF79-59D39A66A975}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:K7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.85546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>114</v>
+      </c>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="24"/>
+    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>121</v>
+      </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+    </row>
+    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="38"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="23"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="36">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="36">
+        <v>2024</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="213.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="36">
+        <v>2023</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="114" x14ac:dyDescent="0.2">
+      <c r="A13" s="36">
+        <v>2022</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>152</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" tooltip="MBLY - Mobileye Global Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=MBLY" xr:uid="{FD61310C-B71E-470A-9660-404E7229D638}"/>
+    <hyperlink ref="C2" r:id="rId2" tooltip="NVDA - NVIDIA Corp Stock Price and Quote" display="https://finviz.com/quote.ashx?t=NVDA" xr:uid="{3DCD4874-8C1C-4989-A2B8-68CFD9C6D6B6}"/>
+    <hyperlink ref="D2" r:id="rId3" tooltip="QCOM - Qualcomm, Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=QCOM" xr:uid="{C6076AFF-E5BE-4036-AB0D-57382F414029}"/>
+    <hyperlink ref="E2" r:id="rId4" tooltip="AMBA - Ambarella Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=AMBA" xr:uid="{61CB2478-1DBB-4720-AAFC-B74F6ABFE077}"/>
+    <hyperlink ref="F2" r:id="rId5" tooltip="APTV - Aptiv PLC Stock Price and Quote" display="https://finviz.com/quote.ashx?t=APTV" xr:uid="{1B8627CC-390D-4D34-8C6C-93CD159FEB18}"/>
+    <hyperlink ref="G2" r:id="rId6" tooltip="BIDU - Baidu Inc ADR Stock Price and Quote" display="https://finviz.com/quote.ashx?t=BIDU" xr:uid="{E1D38789-C4A0-4E3A-B859-83A8ADD1C238}"/>
+    <hyperlink ref="B3" r:id="rId7" tooltip="MBLY - Mobileye Global Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=MBLY" xr:uid="{E973A86F-BED1-4DB9-B25F-AA43FB2BFC86}"/>
+    <hyperlink ref="C3" r:id="rId8" tooltip="NVDA - NVIDIA Corp Stock Price and Quote" display="https://finviz.com/quote.ashx?t=NVDA" xr:uid="{7FB7B454-5217-43D8-9BD7-9C267C01A751}"/>
+    <hyperlink ref="D3" r:id="rId9" tooltip="QCOM - Qualcomm, Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=QCOM" xr:uid="{0472AE30-9314-409B-90F7-6046BE35B9B7}"/>
+    <hyperlink ref="E3" r:id="rId10" tooltip="AMBA - Ambarella Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=AMBA" xr:uid="{9341FCBC-1C8F-4AFE-A87B-4E13204C95AE}"/>
+    <hyperlink ref="F3" r:id="rId11" tooltip="APTV - Aptiv PLC Stock Price and Quote" display="https://finviz.com/quote.ashx?t=APTV" xr:uid="{7CB95D11-A5D6-495A-AC00-218D3062383D}"/>
+    <hyperlink ref="G3" r:id="rId12" tooltip="BIDU - Baidu Inc ADR Stock Price and Quote" display="https://finviz.com/quote.ashx?t=BIDU" xr:uid="{F882AF02-BD09-4AF7-82F0-C4F9CA53460F}"/>
+    <hyperlink ref="B4" r:id="rId13" tooltip="MBLY - Mobileye Global Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=MBLY" xr:uid="{64EE83B4-C1C5-4F2F-BF56-BEDFA3B57A2D}"/>
+    <hyperlink ref="C4" r:id="rId14" tooltip="NVDA - NVIDIA Corp Stock Price and Quote" display="https://finviz.com/quote.ashx?t=NVDA" xr:uid="{5841703E-3248-486E-BE83-5F851282F3AD}"/>
+    <hyperlink ref="D4" r:id="rId15" tooltip="QCOM - Qualcomm, Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=QCOM" xr:uid="{D7221227-10C8-46ED-A50B-9FC3F76093DD}"/>
+    <hyperlink ref="E4" r:id="rId16" tooltip="AMBA - Ambarella Inc Stock Price and Quote" display="https://finviz.com/quote.ashx?t=AMBA" xr:uid="{D12366A3-CD3D-49D4-9DC8-404B816059BC}"/>
+    <hyperlink ref="F4" r:id="rId17" tooltip="APTV - Aptiv PLC Stock Price and Quote" display="https://finviz.com/quote.ashx?t=APTV" xr:uid="{EDF37B76-1B0C-4C8C-8B22-7013CB5B2179}"/>
+    <hyperlink ref="G4" r:id="rId18" tooltip="BIDU - Baidu Inc ADR Stock Price and Quote" display="https://finviz.com/quote.ashx?t=BIDU" xr:uid="{3A3A38ED-27D4-406B-BE0A-C562338CBCAE}"/>
+    <hyperlink ref="C10" r:id="rId19" tooltip="QUALCOMM Incorporated" display="https://s204.q4cdn.com/645488518/files/doc_financials/2025/q4/QCOM-09-28-25-FY2025-10-K-Final.pdf?utm_source=chatgpt.com" xr:uid="{3F8294BB-C820-4C8A-8D6A-73A3A9906AB6}"/>
+    <hyperlink ref="C11" r:id="rId20" tooltip="QUALCOMM Incorporated" display="https://s204.q4cdn.com/645488518/files/doc_financials/2025/q4/QCOM-09-28-25-FY2025-10-K-Final.pdf?utm_source=chatgpt.com" xr:uid="{50DA5D78-0BBB-4C32-A451-F864DF650640}"/>
+    <hyperlink ref="C12" r:id="rId21" tooltip="526bc07f2939fb6478c612a2e77..." display="https://device.report/m/526bc07f2939fb6478c612a2e770c00ec49be1a9f01e54b6419bce82483b31b8_pdf?utm_source=chatgpt.com" xr:uid="{1AB48E11-F440-4B10-894A-ECA5DF8C9E8A}"/>
+    <hyperlink ref="C13" r:id="rId22" tooltip="526bc07f2939fb6478c612a2e77..." display="https://device.report/m/526bc07f2939fb6478c612a2e770c00ec49be1a9f01e54b6419bce82483b31b8_pdf?utm_source=chatgpt.com" xr:uid="{129C9D2F-0DD1-4B51-9F44-4C23C7F4A803}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -3445,31 +3913,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3485,4 +3944,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>